<commit_message>
fixed cell inputs for excel sheet
</commit_message>
<xml_diff>
--- a/homescraper/2024-02-16-house-analysis.xlsx
+++ b/homescraper/2024-02-16-house-analysis.xlsx
@@ -707,11 +707,6 @@
           <t>Yearly</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Yearly</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -730,10 +725,6 @@
         <f>C20*12</f>
         <v/>
       </c>
-      <c r="E20">
-        <f>C20*12</f>
-        <v/>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -752,10 +743,6 @@
         <f>C21*12</f>
         <v/>
       </c>
-      <c r="E21">
-        <f>C21*12</f>
-        <v/>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -764,7 +751,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>174.9</v>
+        <v>0.05</v>
       </c>
       <c r="C22">
         <f>B22*B17</f>
@@ -774,10 +761,6 @@
         <f>C22*12</f>
         <v/>
       </c>
-      <c r="E22">
-        <f>C22*12</f>
-        <v/>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -786,7 +769,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>314.82</v>
+        <v>0.09</v>
       </c>
       <c r="C23">
         <f>B23*B17</f>
@@ -796,10 +779,6 @@
         <f>C23*12</f>
         <v/>
       </c>
-      <c r="E23">
-        <f>C23*12</f>
-        <v/>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -808,7 +787,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>349.8</v>
+        <v>0.1</v>
       </c>
       <c r="C24">
         <f>B24*B17</f>
@@ -818,10 +797,6 @@
         <f>C24*12</f>
         <v/>
       </c>
-      <c r="E24">
-        <f>C24*12</f>
-        <v/>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -830,7 +805,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>349.8</v>
+        <v>0.1</v>
       </c>
       <c r="C25">
         <f>B25*B17</f>
@@ -840,10 +815,6 @@
         <f>C25*12</f>
         <v/>
       </c>
-      <c r="E25">
-        <f>C25*12</f>
-        <v/>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1109,27 +1080,27 @@
         </is>
       </c>
       <c r="B34">
-        <f>((B28/B3)-1)/1</f>
+        <f>((B33+E6)/E6)^(1/(B27+1))-1</f>
         <v/>
       </c>
       <c r="C34">
-        <f>((C33+E6)/E6)^(1/C27)-1</f>
+        <f>((C33+E6)/E6)^(1/(C27+1))-1</f>
         <v/>
       </c>
       <c r="D34">
-        <f>((D33+E6)/E6)^(1/D27)-1</f>
+        <f>((D33+E6)/E6)^(1/(D27+1))-1</f>
         <v/>
       </c>
       <c r="E34">
-        <f>((E33+E6)/E6)^(1/E27)-1</f>
+        <f>((E33+E6)/E6)^(1/(E27+1))-1</f>
         <v/>
       </c>
       <c r="F34">
-        <f>((F33+E6)/E6)^(1/F27)-1</f>
+        <f>((F33+E6)/E6)^(1/(F27+1))-1</f>
         <v/>
       </c>
       <c r="G34">
-        <f>((G33+E6)/E6)^(1/G27)-1</f>
+        <f>((G33+E6)/E6)^(1/(G27+1))-1</f>
         <v/>
       </c>
     </row>
@@ -1435,11 +1406,6 @@
           <t>Yearly</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Yearly</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1458,10 +1424,6 @@
         <f>C20*12</f>
         <v/>
       </c>
-      <c r="E20">
-        <f>C20*12</f>
-        <v/>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1480,10 +1442,6 @@
         <f>C21*12</f>
         <v/>
       </c>
-      <c r="E21">
-        <f>C21*12</f>
-        <v/>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1492,7 +1450,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>113.3</v>
+        <v>0.05</v>
       </c>
       <c r="C22">
         <f>B22*B17</f>
@@ -1502,10 +1460,6 @@
         <f>C22*12</f>
         <v/>
       </c>
-      <c r="E22">
-        <f>C22*12</f>
-        <v/>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1514,7 +1468,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>203.94</v>
+        <v>0.09</v>
       </c>
       <c r="C23">
         <f>B23*B17</f>
@@ -1524,10 +1478,6 @@
         <f>C23*12</f>
         <v/>
       </c>
-      <c r="E23">
-        <f>C23*12</f>
-        <v/>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1536,7 +1486,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>226.6</v>
+        <v>0.1</v>
       </c>
       <c r="C24">
         <f>B24*B17</f>
@@ -1546,10 +1496,6 @@
         <f>C24*12</f>
         <v/>
       </c>
-      <c r="E24">
-        <f>C24*12</f>
-        <v/>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1558,7 +1504,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>226.6</v>
+        <v>0.1</v>
       </c>
       <c r="C25">
         <f>B25*B17</f>
@@ -1568,10 +1514,6 @@
         <f>C25*12</f>
         <v/>
       </c>
-      <c r="E25">
-        <f>C25*12</f>
-        <v/>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1837,27 +1779,27 @@
         </is>
       </c>
       <c r="B34">
-        <f>((B28/B3)-1)/1</f>
+        <f>((B33+E6)/E6)^(1/(B27+1))-1</f>
         <v/>
       </c>
       <c r="C34">
-        <f>((C33+E6)/E6)^(1/C27)-1</f>
+        <f>((C33+E6)/E6)^(1/(C27+1))-1</f>
         <v/>
       </c>
       <c r="D34">
-        <f>((D33+E6)/E6)^(1/D27)-1</f>
+        <f>((D33+E6)/E6)^(1/(D27+1))-1</f>
         <v/>
       </c>
       <c r="E34">
-        <f>((E33+E6)/E6)^(1/E27)-1</f>
+        <f>((E33+E6)/E6)^(1/(E27+1))-1</f>
         <v/>
       </c>
       <c r="F34">
-        <f>((F33+E6)/E6)^(1/F27)-1</f>
+        <f>((F33+E6)/E6)^(1/(F27+1))-1</f>
         <v/>
       </c>
       <c r="G34">
-        <f>((G33+E6)/E6)^(1/G27)-1</f>
+        <f>((G33+E6)/E6)^(1/(G27+1))-1</f>
         <v/>
       </c>
     </row>
@@ -2163,11 +2105,6 @@
           <t>Yearly</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Yearly</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2186,10 +2123,6 @@
         <f>C20*12</f>
         <v/>
       </c>
-      <c r="E20">
-        <f>C20*12</f>
-        <v/>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2208,10 +2141,6 @@
         <f>C21*12</f>
         <v/>
       </c>
-      <c r="E21">
-        <f>C21*12</f>
-        <v/>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2220,7 +2149,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>273.9</v>
+        <v>0.05</v>
       </c>
       <c r="C22">
         <f>B22*B17</f>
@@ -2230,10 +2159,6 @@
         <f>C22*12</f>
         <v/>
       </c>
-      <c r="E22">
-        <f>C22*12</f>
-        <v/>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2242,7 +2167,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>493.02</v>
+        <v>0.09</v>
       </c>
       <c r="C23">
         <f>B23*B17</f>
@@ -2252,10 +2177,6 @@
         <f>C23*12</f>
         <v/>
       </c>
-      <c r="E23">
-        <f>C23*12</f>
-        <v/>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2264,7 +2185,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>547.8</v>
+        <v>0.1</v>
       </c>
       <c r="C24">
         <f>B24*B17</f>
@@ -2274,10 +2195,6 @@
         <f>C24*12</f>
         <v/>
       </c>
-      <c r="E24">
-        <f>C24*12</f>
-        <v/>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2286,7 +2203,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>547.8</v>
+        <v>0.1</v>
       </c>
       <c r="C25">
         <f>B25*B17</f>
@@ -2296,10 +2213,6 @@
         <f>C25*12</f>
         <v/>
       </c>
-      <c r="E25">
-        <f>C25*12</f>
-        <v/>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2565,27 +2478,27 @@
         </is>
       </c>
       <c r="B34">
-        <f>((B28/B3)-1)/1</f>
+        <f>((B33+E6)/E6)^(1/(B27+1))-1</f>
         <v/>
       </c>
       <c r="C34">
-        <f>((C33+E6)/E6)^(1/C27)-1</f>
+        <f>((C33+E6)/E6)^(1/(C27+1))-1</f>
         <v/>
       </c>
       <c r="D34">
-        <f>((D33+E6)/E6)^(1/D27)-1</f>
+        <f>((D33+E6)/E6)^(1/(D27+1))-1</f>
         <v/>
       </c>
       <c r="E34">
-        <f>((E33+E6)/E6)^(1/E27)-1</f>
+        <f>((E33+E6)/E6)^(1/(E27+1))-1</f>
         <v/>
       </c>
       <c r="F34">
-        <f>((F33+E6)/E6)^(1/F27)-1</f>
+        <f>((F33+E6)/E6)^(1/(F27+1))-1</f>
         <v/>
       </c>
       <c r="G34">
-        <f>((G33+E6)/E6)^(1/G27)-1</f>
+        <f>((G33+E6)/E6)^(1/(G27+1))-1</f>
         <v/>
       </c>
     </row>
@@ -2891,11 +2804,6 @@
           <t>Yearly</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Yearly</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2914,10 +2822,6 @@
         <f>C20*12</f>
         <v/>
       </c>
-      <c r="E20">
-        <f>C20*12</f>
-        <v/>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2936,10 +2840,6 @@
         <f>C21*12</f>
         <v/>
       </c>
-      <c r="E21">
-        <f>C21*12</f>
-        <v/>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2948,7 +2848,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>136.9</v>
+        <v>0.05</v>
       </c>
       <c r="C22">
         <f>B22*B17</f>
@@ -2958,10 +2858,6 @@
         <f>C22*12</f>
         <v/>
       </c>
-      <c r="E22">
-        <f>C22*12</f>
-        <v/>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2970,7 +2866,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>246.42</v>
+        <v>0.09</v>
       </c>
       <c r="C23">
         <f>B23*B17</f>
@@ -2980,10 +2876,6 @@
         <f>C23*12</f>
         <v/>
       </c>
-      <c r="E23">
-        <f>C23*12</f>
-        <v/>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2992,7 +2884,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>273.8</v>
+        <v>0.1</v>
       </c>
       <c r="C24">
         <f>B24*B17</f>
@@ -3002,10 +2894,6 @@
         <f>C24*12</f>
         <v/>
       </c>
-      <c r="E24">
-        <f>C24*12</f>
-        <v/>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3014,7 +2902,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>273.8</v>
+        <v>0.1</v>
       </c>
       <c r="C25">
         <f>B25*B17</f>
@@ -3024,10 +2912,6 @@
         <f>C25*12</f>
         <v/>
       </c>
-      <c r="E25">
-        <f>C25*12</f>
-        <v/>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3293,27 +3177,27 @@
         </is>
       </c>
       <c r="B34">
-        <f>((B28/B3)-1)/1</f>
+        <f>((B33+E6)/E6)^(1/(B27+1))-1</f>
         <v/>
       </c>
       <c r="C34">
-        <f>((C33+E6)/E6)^(1/C27)-1</f>
+        <f>((C33+E6)/E6)^(1/(C27+1))-1</f>
         <v/>
       </c>
       <c r="D34">
-        <f>((D33+E6)/E6)^(1/D27)-1</f>
+        <f>((D33+E6)/E6)^(1/(D27+1))-1</f>
         <v/>
       </c>
       <c r="E34">
-        <f>((E33+E6)/E6)^(1/E27)-1</f>
+        <f>((E33+E6)/E6)^(1/(E27+1))-1</f>
         <v/>
       </c>
       <c r="F34">
-        <f>((F33+E6)/E6)^(1/F27)-1</f>
+        <f>((F33+E6)/E6)^(1/(F27+1))-1</f>
         <v/>
       </c>
       <c r="G34">
-        <f>((G33+E6)/E6)^(1/G27)-1</f>
+        <f>((G33+E6)/E6)^(1/(G27+1))-1</f>
         <v/>
       </c>
     </row>

</xml_diff>